<commit_message>
Basic action -> verb flow
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Add more Verb and Primitive definitions</t>
   </si>
   <si>
-    <t xml:space="preserve">Build system for matching ActionEvents to verb/primitive definitions</t>
+    <t xml:space="preserve">Build basic system for matching ActionEvents to verb/primitive definitions</t>
   </si>
   <si>
     <t xml:space="preserve">Implement Object Constraint checks</t>
@@ -58,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,12 +80,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -252,12 +255,12 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -287,7 +290,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Big commit. Started tracking speed, general fixes to CompoundEntities
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -43,7 +43,22 @@
     <t xml:space="preserve">Implement Object Constraint checks</t>
   </si>
   <si>
-    <t xml:space="preserve">Replace “polarity” system with something better</t>
+    <t xml:space="preserve">Make list of possible values for attribute_outcomes for each possible attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add velocity change detection to CompoundEntity.tick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add ‘distance_from_subject’ detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add attribute_outcome types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement "increase/decrease" attribute changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Add 'accelerate' verb</t>
   </si>
 </sst>
 </file>
@@ -90,7 +105,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,19 +115,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC2E0AE"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFADD58A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF9AE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFF685"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7A19A"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF685"/>
+        <bgColor rgb="FFFFF9AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD58A"/>
+        <bgColor rgb="FFC2E0AE"/>
       </patternFill>
     </fill>
   </fills>
@@ -150,7 +177,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,7 +198,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,7 +239,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFF685"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -222,7 +257,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFF9AE"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFADD58A"/>
       <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -252,15 +287,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -300,8 +335,33 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support for 'attribute outcome' added
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
   <si>
+    <t xml:space="preserve">Done?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Change “CDConverter” to output ActionEvents</t>
   </si>
   <si>
@@ -52,13 +55,34 @@
     <t xml:space="preserve">Add ‘distance_from_subject’ detection</t>
   </si>
   <si>
-    <t xml:space="preserve">Add attribute_outcome types</t>
+    <t xml:space="preserve">Setup attribute_outcome enum</t>
   </si>
   <si>
     <t xml:space="preserve">implement "increase/decrease" attribute changes</t>
   </si>
   <si>
-    <t xml:space="preserve">*Add 'accelerate' verb</t>
+    <t xml:space="preserve">Add 'accelerate' verb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make initial list of object constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build a plan for complex scenarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new ComplexEntity when an object is expelled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create distance ‘matrix’ for distances between objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store objects’ event histories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add support for merging objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log objects’ propelling each other</t>
   </si>
 </sst>
 </file>
@@ -68,12 +92,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="19">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,25 +115,155 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <strike val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="10"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFF9AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC2E0AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -121,7 +274,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF9AE"/>
-        <bgColor rgb="FFFFF685"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -143,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -151,8 +304,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,75 +344,174 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="25">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Strikethrough" xfId="37" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="De-emphasised Strikethrough" xfId="38" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <family val="2"/>
+        <strike val="1"/>
+        <color rgb="FF999999"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFF685"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC2E0AE"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFF685"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -260,7 +527,7 @@
       <rgbColor rgb="FFADD58A"/>
       <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -268,7 +535,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -287,10 +554,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -303,68 +570,144 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>8</v>
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>10</v>
+      <c r="A11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>12</v>
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A100">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$B2=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B20" type="whole">
+      <formula1>2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Logging distances between objects
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -557,7 +557,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,6 +679,9 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>17</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Writing up background of CD theory
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Programming" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Writing" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Structure" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -89,6 +91,39 @@
   </si>
   <si>
     <t xml:space="preserve">Build system to inject arbitary object into simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle radius changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add attribute outcome to CD events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read example dissertations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read papers on CD/Metaphor stuff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write more detail on implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Literature Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusion + Future Work</t>
   </si>
 </sst>
 </file>
@@ -213,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,6 +291,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -351,10 +390,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -504,6 +543,22 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>22</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -526,4 +581,121 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A1000">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$B2=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of compound CDEvents, queueing
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t xml:space="preserve">Basic Preposition Support (‘into’)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test CD definition with previous events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Verb→CD converter to output array (if applicable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set parse_sentence to output array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change setup_pymunk_environment to setup queued events</t>
   </si>
   <si>
     <t xml:space="preserve">Read example dissertations</t>
@@ -402,10 +414,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,6 +609,29 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +683,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -656,12 +691,12 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -699,32 +734,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logs event history, applies queueing of events for complex CD events
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t xml:space="preserve">Change setup_pymunk_environment to setup queued events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process queued event type tuples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recognise injest/expel events for big particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify ‘get_inclusion_radius’ for single particle/large particle entities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find out if we’re recording distances between objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check which entities are within inclusion radius</t>
   </si>
   <si>
     <t xml:space="preserve">Read example dissertations</t>
@@ -157,12 +172,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="18">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,25 +195,142 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <strike val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFF9AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC2E0AE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -210,7 +341,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF9AE"/>
-        <bgColor rgb="FFFFF685"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -233,12 +364,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF999999"/>
+        <fgColor rgb="FFFFF450"/>
+        <bgColor rgb="FFFFF685"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -246,8 +377,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -271,45 +417,104 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,24 +522,52 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
       <font>
         <name val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <strike val="1"/>
         <color rgb="FF999999"/>
@@ -350,31 +583,31 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFF450"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC2E0AE"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFF685"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF685"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -387,7 +620,7 @@
       <rgbColor rgb="FFADD58A"/>
       <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -414,224 +647,283 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B18" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="B25" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -640,9 +932,13 @@
       <formula>$B2=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B20" type="whole">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1" type="whole">
       <formula1>2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B37" type="list">
+      <formula1>"1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -674,29 +970,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>33</v>
+      <c r="A2" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>34</v>
+      <c r="A3" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>35</v>
+      <c r="A4" s="16" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -734,32 +1030,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>